<commit_message>
Collect storage areas read & write at code element level : OK
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/SymbolInformationsAndStorageAreas.xlsx
+++ b/TypeCobol/Documentation/Studies/SymbolInformationsAndStorageAreas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Desktop\TypeCobol sudies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Laurent\OneDrive\Dev\Github\TypeCobol\TypeCobol\Documentation\Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="5535" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11580" windowHeight="5535" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SymbolInformation" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="315">
   <si>
     <t>SymbolDefinition</t>
   </si>
@@ -342,12 +342,6 @@
     <t>CreateOtherStorageAreaReference</t>
   </si>
   <si>
-    <t>CreateIntegerVariable</t>
-  </si>
-  <si>
-    <t>CreateIntegerVariableOrIndex</t>
-  </si>
-  <si>
     <t>CreateCharacterVariable</t>
   </si>
   <si>
@@ -397,9 +391,6 @@
   </si>
   <si>
     <t>CreateMethodNameVariable</t>
-  </si>
-  <si>
-    <t>CreateVariableOrExpression</t>
   </si>
   <si>
     <t>CreateNumericStorageArea</t>
@@ -1076,6 +1067,42 @@
 - identifier-5 and the corresponding PROCEDURE DIVISION RETURNING identifier in the target program must have the same PICTURE, USAGE, SIGN, SYNCHRONIZE, JUSTIFIED, and BLANK WHEN ZERO clauses (except that PICTURE clause currency symbols can differ, and periods and commas can be interchanged due to the DECIMAL POINT IS COMMA clause).
 When the target returns, its return value is assigned to identifier-5 using the rules for the SET statement if identifier-6 is of usage INDEX, POINTER, FUNCTION-POINTER, PROCEDURE-POINTER, or OBJECT REFERENCE.
 When identifier-5 is of any other usage, the rules for the MOVE statement are used.</t>
+  </si>
+  <si>
+    <t>CreateConditionStorageArea</t>
+  </si>
+  <si>
+    <t>TO DO for write :</t>
+  </si>
+  <si>
+    <t>TO DO for read :</t>
+  </si>
+  <si>
+    <t>CreateIntegerVariable(var 2)</t>
+  </si>
+  <si>
+    <t>CreateIntegerVariable(var 1)</t>
+  </si>
+  <si>
+    <t>CreateIntegerVariableOrIndex(var 1)</t>
+  </si>
+  <si>
+    <t>CreateIntegerVariableOrIndex(var 2)</t>
+  </si>
+  <si>
+    <t>CreateVariable(var7)</t>
+  </si>
+  <si>
+    <t>MoveSimpleStatement</t>
+  </si>
+  <si>
+    <t>CreateVariableOrExpression(var 1)</t>
+  </si>
+  <si>
+    <t>CreateVariableOrExpression(var 2)</t>
+  </si>
+  <si>
+    <t>CreateEvaluateSelectionSubject</t>
   </si>
 </sst>
 </file>
@@ -1223,7 +1250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1248,9 +1275,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1323,6 +1348,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2182,22 +2208,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2207,27 +2233,27 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>226</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2237,17 +2263,17 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2257,12 +2283,12 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2272,12 +2298,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2287,22 +2313,22 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2312,10 +2338,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H172"/>
+  <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="B157" sqref="B157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2332,12 +2358,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2347,7 +2373,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2356,18 +2382,18 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="21" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="23" t="s">
-        <v>108</v>
-      </c>
-    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="23" t="s">
-        <v>109</v>
+      <c r="C10" s="21" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2377,823 +2403,918 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="32" t="s">
-        <v>114</v>
-      </c>
-    </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="16" t="s">
-        <v>165</v>
-      </c>
-    </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="D18" s="16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>135</v>
-      </c>
-    </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>136</v>
+      <c r="C20" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E21" s="19" t="s">
-        <v>103</v>
+      <c r="D21" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
+      <c r="E22" s="19" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E25" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G23" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E24" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F25" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G26" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="14" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H28" s="14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E29" s="19" t="s">
-        <v>138</v>
+      <c r="H29" s="14" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F30" t="s">
-        <v>146</v>
+      <c r="E30" s="19" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G31" t="s">
-        <v>147</v>
+      <c r="F31" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H34" s="14" t="s">
-        <v>150</v>
+      <c r="G34" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E35" s="21" t="s">
+      <c r="H35" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E36" s="20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F36" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G37" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G38" s="2" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G39" s="2" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="G40" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E44" s="22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F45" s="21" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E43" s="24" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F44" s="23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C46" t="s">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E48" s="19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C51" s="15" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C52" s="15" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C53" s="15" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C54" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C55" s="15" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="28" t="s">
+      <c r="C56" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="26" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="25"/>
+      <c r="C58" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="24"/>
+      <c r="C59" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E59" s="28"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="26" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="25"/>
+      <c r="C61" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="29" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="25"/>
+      <c r="C63" s="14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="26" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="27"/>
-      <c r="C57" s="14" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="25"/>
+      <c r="C65" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="58" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="26"/>
-      <c r="C58" s="30" t="s">
+    <row r="66" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="E58" s="30"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="27"/>
-      <c r="C60" s="4" t="s">
+    </row>
+    <row r="67" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="25"/>
+      <c r="C67" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="25"/>
+      <c r="C69" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E69" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="C70" s="22"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="31"/>
+      <c r="C71" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="31"/>
+      <c r="C72" s="21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="31"/>
+      <c r="C73" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="20" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="31" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="27"/>
-      <c r="C62" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="27"/>
-      <c r="C64" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="28" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="27"/>
-      <c r="C66" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="27"/>
-      <c r="C68" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="E68" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="C69" s="24"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="33"/>
-      <c r="C70" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="33"/>
-      <c r="C71" s="23" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C77" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="33"/>
-      <c r="C72" s="23" t="s">
+    <row r="79" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="21" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="33" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B80" s="15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C84" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C88" s="15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="35" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="19" t="s">
-        <v>116</v>
-      </c>
-    </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C92" s="32" t="s">
+      <c r="B92" s="19" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="19" t="s">
-        <v>102</v>
+      <c r="C93" s="30" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C94" s="14" t="s">
-        <v>163</v>
+      <c r="B94" s="19" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C95" s="14" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C96" s="14" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C97" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="14" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="19" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C99" s="36" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C101" s="14" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C102" s="14" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C103" s="14" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C104" s="14" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C105" s="14" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C106" s="14" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C107" s="14" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C108" s="14" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C109" s="14" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C110" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C111" s="14" t="s">
-        <v>184</v>
+        <v>139</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="19" t="s">
-        <v>173</v>
+      <c r="C112" s="14" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C113" s="14" t="s">
-        <v>185</v>
+      <c r="B113" s="19" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C114" s="14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C115" s="14" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B116" s="19" t="s">
-        <v>174</v>
+      <c r="C116" s="14" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C117" s="14" t="s">
-        <v>185</v>
+      <c r="B117" s="19" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C118" s="14" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C119" s="14" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B120" s="19" t="s">
+      <c r="C120" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D121" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C122" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C124" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="D120" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C121" s="14" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B122" s="19" t="s">
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C126" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C123" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B124" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C125" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B126" s="19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C127" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B128" s="19" t="s">
-        <v>190</v>
+      <c r="C128" s="14" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C129" s="14" t="s">
-        <v>194</v>
+      <c r="B129" s="19" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C130" s="14" t="s">
-        <v>195</v>
+      <c r="B130" s="30"/>
+      <c r="C130" s="30" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C131" s="14" t="s">
-        <v>196</v>
+      <c r="B131" s="30"/>
+      <c r="C131" s="30" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C132" s="14" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C133" s="14" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C134" s="14" t="s">
-        <v>168</v>
+      <c r="B134" s="30"/>
+      <c r="C134" s="30" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C135" s="14" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C136" s="14" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C137" s="14" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B138" s="24" t="s">
-        <v>191</v>
+      <c r="C138" s="14" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C139" s="13" t="s">
-        <v>130</v>
+      <c r="C139" s="14" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B140" s="19" t="s">
-        <v>192</v>
+      <c r="C140" s="14" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C141" s="14" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C142" s="14" t="s">
-        <v>201</v>
+      <c r="B142" s="22" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C143" s="14" t="s">
-        <v>202</v>
+      <c r="C143" s="13" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="19" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C145" s="14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C146" s="14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C147" s="14" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B148" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C149" s="14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C150" s="14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="18"/>
+      <c r="C152" s="14" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="C153" s="19"/>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C154" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D155" s="14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="13" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C146" s="14" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B147" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C147" s="19"/>
-    </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C148" t="s">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="D157" s="13"/>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C158" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="D158" s="13"/>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="32" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="6"/>
+      <c r="C160" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D149" s="14" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D150" s="13" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B151" s="34" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B152" s="6"/>
-      <c r="C152" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B153" s="6"/>
-      <c r="C153" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B154" s="6"/>
-      <c r="C154" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B155" s="34" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B156" s="6"/>
-      <c r="C156" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B157" s="6"/>
-      <c r="C157" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B158" s="6"/>
-      <c r="C158" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E158" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="F158" s="9"/>
-      <c r="G158" s="9"/>
-    </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B159" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="C159" s="24"/>
-    </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B160" s="6"/>
-      <c r="C160" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B161" s="6"/>
       <c r="C161" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
-      <c r="C162" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B163" s="6"/>
-      <c r="C163" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C162" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B163" s="32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
       <c r="C164" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B165" s="6"/>
       <c r="C165" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
       <c r="C166" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B167" s="6"/>
-      <c r="C167" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C168" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="E166" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="F166" s="9"/>
+      <c r="G166" s="9"/>
+    </row>
+    <row r="167" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B167" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="C167" s="22"/>
+    </row>
+    <row r="168" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B168" s="6"/>
+      <c r="C168" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B169" s="6"/>
       <c r="C169" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B170" s="22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B171" s="22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B172" s="22" t="s">
-        <v>126</v>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B170" s="6"/>
+      <c r="C170" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B171" s="6"/>
+      <c r="C171" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B172" s="6"/>
+      <c r="C172" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B173" s="6"/>
+      <c r="C173" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B174" s="6"/>
+      <c r="C174" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B175" s="6"/>
+      <c r="C175" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C176" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="21" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B188" s="22"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B189" s="22"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="B193" s="19"/>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="22" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3214,37 +3335,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>219</v>
+      <c r="A8" s="27" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3256,481 +3377,481 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="37" customWidth="1"/>
-    <col min="2" max="2" width="16.375" style="37" customWidth="1"/>
-    <col min="3" max="3" width="59.375" style="37" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="37"/>
+    <col min="1" max="1" width="18.5" style="35" customWidth="1"/>
+    <col min="2" max="2" width="16.375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="59.375" style="35" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="37"/>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="38"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>232</v>
+      </c>
+      <c r="B9" s="39"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="40" t="s">
+        <v>245</v>
+      </c>
+      <c r="B10" s="40"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="35" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" s="40" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+    </row>
+    <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>234</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="35" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" s="39"/>
+      <c r="C22" s="38" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="37"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="35" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="37"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="38" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="37"/>
+      <c r="B25" s="37"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="37"/>
+      <c r="B27" s="37"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="B28" s="37"/>
+    </row>
+    <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="C29" s="38" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>230</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="B35" s="37"/>
+    </row>
+    <row r="36" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="C36" s="38" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="C37" s="48" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="C38" s="49" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="35" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="C42" s="43" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="C43" s="49" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="35" t="s">
+        <v>277</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="43"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
+        <v>299</v>
+      </c>
+      <c r="C46" s="54" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A47" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" s="38" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="B2" s="39"/>
-    </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40" t="s">
+      <c r="B49" s="37"/>
+    </row>
+    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="C50" s="38" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="40" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="40" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="40"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
-        <v>235</v>
-      </c>
-      <c r="B9" s="41"/>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
-        <v>248</v>
-      </c>
-      <c r="B10" s="42"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="37" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="42"/>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
-      <c r="B13" s="42" t="s">
-        <v>233</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
-      <c r="B14" s="42" t="s">
-        <v>249</v>
-      </c>
-      <c r="C14" s="44" t="s">
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="C52" s="38" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="42"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-    </row>
-    <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
-        <v>234</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>234</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="s">
-        <v>237</v>
-      </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="37" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
-        <v>238</v>
-      </c>
-      <c r="B22" s="41"/>
-      <c r="C22" s="40" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="37" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="40" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="39"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="39"/>
-      <c r="B26" s="39"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="B27" s="39"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="39" t="s">
-        <v>240</v>
-      </c>
-      <c r="B28" s="39"/>
-    </row>
-    <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C29" s="40" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="37" t="s">
-        <v>233</v>
-      </c>
-      <c r="C32" s="43" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="C33" s="43" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
-        <v>241</v>
-      </c>
-      <c r="B35" s="39"/>
-    </row>
-    <row r="36" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C36" s="40" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C37" s="50" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="35" t="s">
+        <v>231</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="37" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="47" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="44" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="47" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="44" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="47" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="44" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="44" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="44" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="45" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="46" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="43" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="43" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="35" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="35" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="35" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="35" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="35" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="B79" s="53" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="50" t="s">
+        <v>289</v>
+      </c>
+      <c r="B81" s="50" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="52" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="C82" s="52" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="52" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="C83" s="52" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" s="52" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="C84" s="52" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" s="52" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="C85" s="52" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="51" t="s">
+        <v>286</v>
+      </c>
+      <c r="B87" s="51" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="51" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="35" t="s">
+        <v>281</v>
+      </c>
+      <c r="B90" s="35" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C38" s="51" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="37" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="C42" s="45" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="C43" s="51" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="37" t="s">
-        <v>280</v>
-      </c>
-      <c r="C44" s="45" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C45" s="45"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="37" t="s">
-        <v>302</v>
-      </c>
-      <c r="C46" s="56" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="C47" s="40" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="39" t="s">
-        <v>242</v>
-      </c>
-      <c r="B49" s="39"/>
-    </row>
-    <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C50" s="40" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="C52" s="40" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="B53" s="37" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="39" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="46" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="49" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="46" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="49" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="46" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="46" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="46" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="47" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="48" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="45" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="45" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="37" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="37" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="37" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="37" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="55" t="s">
-        <v>286</v>
-      </c>
-      <c r="B79" s="55" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="52" t="s">
-        <v>292</v>
-      </c>
-      <c r="B81" s="52" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" s="54" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="C82" s="54" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" s="54" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="C83" s="54" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" s="54" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="C84" s="54" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" s="54" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="C85" s="54" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" s="52" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:3" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="53" t="s">
-        <v>289</v>
-      </c>
-      <c r="B87" s="53" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="53" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="37" t="s">
-        <v>284</v>
-      </c>
-      <c r="B90" s="37" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="35" t="s">
         <v>285</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="37" t="s">
-        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepare to collect CallTargetParameters and CallSiteParameters
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/SymbolInformationsAndStorageAreas.xlsx
+++ b/TypeCobol/Documentation/Studies/SymbolInformationsAndStorageAreas.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="346">
   <si>
     <t>SymbolDefinition</t>
   </si>
@@ -1103,6 +1103,99 @@
   </si>
   <si>
     <t>CreateEvaluateSelectionSubject</t>
+  </si>
+  <si>
+    <t>statement.OutputParameter = CobolExpressionsBuilder.CreateStorageArea(context.callProgramOutputParameter().storageArea1());</t>
+  </si>
+  <si>
+    <t>var inputParameter = new CallInputParameter { SendingMode = sendingMode };</t>
+  </si>
+  <si>
+    <t>CobolExpressionsBuilder.CreateVariable(variableContext));</t>
+  </si>
+  <si>
+    <t>statement.InputParameters.Add(CobolExpressionsBuilder.CreateVariable(variableContext));</t>
+  </si>
+  <si>
+    <t>statement.OutputParameter = cobolExpressionsBuilder.CreateStorageArea(context.invokeOutputParameter().storageArea1());</t>
+  </si>
+  <si>
+    <t>inputParameter.SendingVariable = cobolExpressionsBuilder.CreateVariableOrFileName(variable.variableOrFileName());</t>
+  </si>
+  <si>
+    <t>arguments[i] = CreateVariableOrExpression(argumentContext[i].variableOrExpression1())</t>
+  </si>
+  <si>
+    <t>EnterProcedureDivisionHeader</t>
+  </si>
+  <si>
+    <t>&gt; EnterReturningPhrase</t>
+  </si>
+  <si>
+    <t>&gt; CreateInputParameters</t>
+  </si>
+  <si>
+    <t>CreateEntryStatement</t>
+  </si>
+  <si>
+    <t>statement.InputParameters = CreateInputParameters(context.programInputParameters());</t>
+  </si>
+  <si>
+    <t>((Returning)CodeElement).ReturningParameter = CobolExpressionsBuilder.CreateStorageArea(context.programOutputParameter().storageArea2());</t>
+  </si>
+  <si>
+    <t>var inputParameter = new InputParameter (receivingMode, CobolExpressionsBuilder.CreateStorageArea(storageAreaContext);</t>
+  </si>
+  <si>
+    <t>&gt; CallInputParameter / VariableOrFileName</t>
+  </si>
+  <si>
+    <t>&gt; ReceivingStorageArea</t>
+  </si>
+  <si>
+    <t>&gt; VariableOrExpression</t>
+  </si>
+  <si>
+    <t>&gt; Variable</t>
+  </si>
+  <si>
+    <t>EnterFunctionDeclarationHeader</t>
+  </si>
+  <si>
+    <t>var ce = (FunctionDeclarationHeader)CodeElement;</t>
+  </si>
+  <si>
+    <t>ce.Input = new SyntaxProperty&lt;Passing.Mode&gt;(Passing.Mode.Input, ParseTreeUtils.GetTokenFromTerminalNode(context.INPUT()));</t>
+  </si>
+  <si>
+    <t>ce.Profile.InputParameters = CreateParameters(context.parameterDescription());</t>
+  </si>
+  <si>
+    <t>&gt; CreateArguments</t>
+  </si>
+  <si>
+    <t>&gt;  CreateFunctionDataParameter</t>
+  </si>
+  <si>
+    <t>&gt; Passing.Mode</t>
+  </si>
+  <si>
+    <t>&gt; ParametersProfile</t>
+  </si>
+  <si>
+    <t>&gt; ParameterDescriptionEntry</t>
+  </si>
+  <si>
+    <t>&gt; DataDescriptionEntry</t>
+  </si>
+  <si>
+    <t>&gt; ReceivingMode</t>
+  </si>
+  <si>
+    <t>&gt; InputParameter</t>
+  </si>
+  <si>
+    <t>&gt; SendingMode</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1349,6 +1442,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2338,10 +2434,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H194"/>
+  <dimension ref="A1:J220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="B200" sqref="B200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3254,66 +3350,234 @@
         <v>165</v>
       </c>
     </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="13" t="s">
+        <v>322</v>
+      </c>
+    </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="13" t="s">
+      <c r="A181" s="56" t="s">
+        <v>324</v>
+      </c>
+      <c r="C181" s="57" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="56" t="s">
+        <v>323</v>
+      </c>
+      <c r="C182" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="56" t="s">
+        <v>325</v>
+      </c>
+      <c r="C183" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="56"/>
+      <c r="B184" s="58" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="56"/>
+      <c r="B185" s="58" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="56"/>
+      <c r="B186" s="58" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="56"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="56" t="s">
+        <v>333</v>
+      </c>
+      <c r="C188" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="56"/>
+      <c r="C189" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="56"/>
+      <c r="C190" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="56" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="56"/>
+      <c r="B192" s="58" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" s="56"/>
+      <c r="B193" s="58" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194" s="56"/>
+      <c r="B194" s="58" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195" s="56"/>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" s="13" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="13" t="s">
+      <c r="C196" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C197" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" s="13"/>
+      <c r="C198" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A199" s="13"/>
+      <c r="B199" s="58" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A200" s="13"/>
+      <c r="B200" s="58" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201" s="13"/>
+      <c r="B201" s="58" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" s="13"/>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" s="13" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="13" t="s">
+      <c r="C203" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" s="13"/>
+      <c r="C204" t="s">
+        <v>319</v>
+      </c>
+      <c r="J204" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205" s="13"/>
+      <c r="B205" s="58" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206" s="13"/>
+      <c r="B206" s="58" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207" s="13"/>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" s="13" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="21" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="C209" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="13"/>
+      <c r="B210" s="58" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="13"/>
+      <c r="B211" s="58" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="32" t="s">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="B188" s="22"/>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" s="32" t="s">
+      <c r="B214" s="22"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="B189" s="22"/>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
+      <c r="B215" s="22"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="22" t="s">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="22" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A193" s="22" t="s">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="B193" s="19"/>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A194" s="22" t="s">
+      <c r="B219" s="19"/>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="22" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Separate in grammar : read/write storage areas and shared storage areas between caller and callee
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/SymbolInformationsAndStorageAreas.xlsx
+++ b/TypeCobol/Documentation/Studies/SymbolInformationsAndStorageAreas.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="369">
   <si>
     <t>SymbolDefinition</t>
   </si>
@@ -1197,12 +1197,81 @@
   <si>
     <t>&gt; SendingMode</t>
   </si>
+  <si>
+    <t>variableOrFileName | OMITTED;</t>
+  </si>
+  <si>
+    <t>callProgramOutputParameter:</t>
+  </si>
+  <si>
+    <t>storageArea1;</t>
+  </si>
+  <si>
+    <t>invokeOutputParameter:</t>
+  </si>
+  <si>
+    <t>=&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variableOrFileNameOrOmitted: </t>
+  </si>
+  <si>
+    <t>sharedVariableOrFileName | OMITTED;</t>
+  </si>
+  <si>
+    <t>invokeInputParameter:</t>
+  </si>
+  <si>
+    <t>BY? VALUE sharedVariable3+;</t>
+  </si>
+  <si>
+    <t>BY? VALUE variable3+;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">argument: </t>
+  </si>
+  <si>
+    <t>variableOrExpression1;</t>
+  </si>
+  <si>
+    <t>sharedVariableOrExpression1;</t>
+  </si>
+  <si>
+    <t>programInputParameters:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    (BY? (REFERENCE | VALUE))? sharedStorageArea2+;</t>
+  </si>
+  <si>
+    <t>programOutputParameter:</t>
+  </si>
+  <si>
+    <t>sharedStorageArea2;</t>
+  </si>
+  <si>
+    <t>sharedStorageArea1</t>
+  </si>
+  <si>
+    <t>CreateSharedVariable(var3)</t>
+  </si>
+  <si>
+    <t>CreateSharedVariableOrFileName</t>
+  </si>
+  <si>
+    <t>CreateSharedStorageArea(st2)</t>
+  </si>
+  <si>
+    <t>CreateSharedVariableOrExpression(var 1)</t>
+  </si>
+  <si>
+    <t>CreateSharedStorageArea(st1)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1280,8 +1349,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1330,6 +1413,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1343,7 +1432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1369,7 +1458,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1445,6 +1533,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2337,8 +2429,8 @@
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
+    <row r="10" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="22" t="s">
         <v>223</v>
       </c>
     </row>
@@ -2434,10 +2526,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J220"/>
+  <dimension ref="A1:J242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="B200" sqref="B200"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2478,17 +2570,17 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="60" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="60" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="60" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2503,18 +2595,18 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="29" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="31" t="s">
         <v>303</v>
       </c>
-      <c r="D14" s="30"/>
+      <c r="D14" s="29"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="55" t="s">
+      <c r="D15" s="54" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2659,12 +2751,12 @@
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E44" s="22" t="s">
-        <v>130</v>
+      <c r="E44" s="21" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F45" s="21" t="s">
+      <c r="F45" s="55" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2724,590 +2816,587 @@
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="26" t="s">
+      <c r="B57" s="25" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="25"/>
+      <c r="B58" s="24"/>
       <c r="C58" s="14" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="59" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="24"/>
-      <c r="C59" s="28" t="s">
+      <c r="B59" s="23"/>
+      <c r="C59" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="E59" s="28"/>
+      <c r="E59" s="27"/>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="26" t="s">
+      <c r="B60" s="25" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="25"/>
+      <c r="B61" s="24"/>
       <c r="C61" s="4" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="29" t="s">
+      <c r="B62" s="28" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="25"/>
+      <c r="B63" s="24"/>
       <c r="C63" s="14" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="26" t="s">
+      <c r="B64" s="25" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="25"/>
+      <c r="B65" s="24"/>
       <c r="C65" s="14" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="66" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="26" t="s">
+      <c r="B66" s="25" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="25"/>
+      <c r="B67" s="24"/>
       <c r="C67" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="26" t="s">
+      <c r="B68" s="25" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="25"/>
-      <c r="C69" s="30" t="s">
+      <c r="B69" s="24"/>
+      <c r="C69" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="E69" s="28" t="s">
+      <c r="E69" s="27" t="s">
         <v>155</v>
       </c>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="32" t="s">
+      <c r="B70" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="C70" s="22"/>
+      <c r="C70" s="18"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="31"/>
+      <c r="B71" s="30"/>
       <c r="C71" s="2" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="31"/>
-      <c r="C72" s="21" t="s">
+      <c r="B72" s="61" t="s">
+        <v>366</v>
+      </c>
+      <c r="C72" s="18"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="30"/>
+      <c r="C73" s="55" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="31"/>
-      <c r="C73" s="21" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="30"/>
+      <c r="C74" s="55" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="75" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
+    <row r="76" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B76" s="20" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="20" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="2" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C78" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
+    <row r="80" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="15" t="s">
+    <row r="81" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="15" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="15" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="15" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
+    <row r="84" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C85" s="15" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
+    <row r="88" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C89" s="15" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="15" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="33" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="32" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="19" t="s">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="19" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C93" s="30" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="29" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="19" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="19" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C95" s="14" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C96" s="14" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C97" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C98" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="19" t="s">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C100" s="34" t="s">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="33" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="19" t="s">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="19" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C102" s="14" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C103" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C104" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C105" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C106" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C107" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C108" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C109" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C110" s="14" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C111" s="14" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C112" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C113" s="14" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="19" t="s">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="19" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C114" s="14" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C115" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C116" s="14" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B117" s="19" t="s">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="19" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C118" s="14" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C119" s="14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C120" s="14" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C121" s="14" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B121" s="19" t="s">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D122" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C122" s="14" t="s">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C123" s="14" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B123" s="19" t="s">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C124" s="14" t="s">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C125" s="14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B125" s="19" t="s">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="19" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C126" s="14" t="s">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C127" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B127" s="19" t="s">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C128" s="14" t="s">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B129" s="19" t="s">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B130" s="19" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B130" s="30"/>
-      <c r="C130" s="30" t="s">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B131" s="29"/>
+      <c r="C131" s="29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B131" s="30"/>
-      <c r="C131" s="30" t="s">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" s="29"/>
+      <c r="C132" s="29" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C132" s="14" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C133" s="14" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="14" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B134" s="30"/>
-      <c r="C134" s="30" t="s">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135" s="29"/>
+      <c r="C135" s="29" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C135" s="14" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C136" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C137" s="14" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C138" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C139" s="14" t="s">
-        <v>195</v>
+        <v>165</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C140" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C141" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B142" s="22" t="s">
-        <v>188</v>
-      </c>
-    </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C143" s="13" t="s">
+      <c r="B143" s="21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="13" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="19" t="s">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" s="19" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C145" s="14" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C146" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C147" s="14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C148" s="14" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="19" t="s">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B149" s="19" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C149" s="14" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C150" s="14" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C151" s="14" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B151" s="19" t="s">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="19" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B152" s="18"/>
-      <c r="C152" s="14" t="s">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="18"/>
+      <c r="C153" s="14" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B153" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="C153" s="19"/>
-    </row>
     <row r="154" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C154" t="s">
+      <c r="B154" s="21" t="s">
+        <v>367</v>
+      </c>
+      <c r="C154" s="18"/>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C155" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D155" s="14" t="s">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D156" s="55" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D156" s="13" t="s">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D157" s="13" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="19" t="s">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D158" s="13"/>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="D157" s="13"/>
-    </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C158" s="14" t="s">
+      <c r="D159" s="13"/>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C160" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="D158" s="13"/>
-    </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B159" s="32" t="s">
+      <c r="D160" s="13"/>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B161" s="31" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B160" s="6"/>
-      <c r="C160" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="161" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B161" s="6"/>
-      <c r="C161" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="162" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
       <c r="C162" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="163" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B163" s="32" t="s">
-        <v>120</v>
+      <c r="B163" s="6"/>
+      <c r="C163" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="164" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B164" s="6"/>
       <c r="C164" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="165" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B165" s="6"/>
-      <c r="C165" s="2" t="s">
-        <v>207</v>
+      <c r="B165" s="31" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="166" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B166" s="6"/>
       <c r="C166" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E166" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="F166" s="9"/>
-      <c r="G166" s="9"/>
+        <v>206</v>
+      </c>
     </row>
     <row r="167" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B167" s="32" t="s">
-        <v>209</v>
-      </c>
-      <c r="C167" s="22"/>
+      <c r="B167" s="6"/>
+      <c r="C167" s="2" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="168" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B168" s="6"/>
-      <c r="C168" s="13" t="s">
-        <v>131</v>
-      </c>
+      <c r="C168" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E168" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="F168" s="9"/>
+      <c r="G168" s="9"/>
     </row>
     <row r="169" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B169" s="6"/>
-      <c r="C169" s="2" t="s">
-        <v>211</v>
-      </c>
+      <c r="B169" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="C169" s="18"/>
     </row>
     <row r="170" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B170" s="6"/>
-      <c r="C170" s="13" t="s">
-        <v>127</v>
+      <c r="C170" s="2" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="171" spans="2:7" x14ac:dyDescent="0.25">
@@ -3350,235 +3439,366 @@
         <v>165</v>
       </c>
     </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B178" s="61" t="s">
+        <v>368</v>
+      </c>
+      <c r="C178" s="18"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B179" s="6"/>
+      <c r="C179" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="13" t="s">
+      <c r="B180" s="6"/>
+      <c r="C180" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="13" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" s="56" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="55" t="s">
         <v>324</v>
       </c>
-      <c r="C181" s="57" t="s">
+      <c r="C183" s="56" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" s="56" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="55" t="s">
         <v>323</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C184" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" s="56" t="s">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="55" t="s">
         <v>325</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C185" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" s="56"/>
-      <c r="B184" s="58" t="s">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="55"/>
+      <c r="B186" s="57" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" s="56"/>
-      <c r="B185" s="58" t="s">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="55"/>
+      <c r="B187" s="57" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="56"/>
-      <c r="B186" s="58" t="s">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="55"/>
+      <c r="B188" s="57" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" s="56"/>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" s="56" t="s">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="55"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="55" t="s">
         <v>333</v>
       </c>
-      <c r="C188" t="s">
+      <c r="C190" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" s="56"/>
-      <c r="C189" t="s">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="55"/>
+      <c r="C191" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" s="56"/>
-      <c r="C190" t="s">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="55"/>
+      <c r="C192" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" s="56" t="s">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" s="55" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A192" s="56"/>
-      <c r="B192" s="58" t="s">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A194" s="55"/>
+      <c r="B194" s="57" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A193" s="56"/>
-      <c r="B193" s="58" t="s">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A195" s="55"/>
+      <c r="B195" s="57" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A194" s="56"/>
-      <c r="B194" s="58" t="s">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A196" s="55"/>
+      <c r="B196" s="57" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A195" s="56"/>
-    </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A196" s="13" t="s">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197" s="55"/>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A198" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="C196" t="s">
+      <c r="C198" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C197" t="s">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C199" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A198" s="13"/>
-      <c r="C198" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A199" s="13"/>
-      <c r="B199" s="58" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="13"/>
-      <c r="B200" s="58" t="s">
-        <v>329</v>
+      <c r="C200" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
-      <c r="B201" s="58" t="s">
-        <v>330</v>
+      <c r="B201" s="57" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="13"/>
+      <c r="B202" s="57" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A203" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C203" t="s">
-        <v>318</v>
+      <c r="A203" s="13"/>
+      <c r="B203" s="57" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="13"/>
-      <c r="C204" t="s">
-        <v>319</v>
-      </c>
-      <c r="J204" t="s">
-        <v>317</v>
-      </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A205" s="13"/>
-      <c r="B205" s="58" t="s">
-        <v>332</v>
+      <c r="A205" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C205" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="13"/>
-      <c r="B206" s="58" t="s">
-        <v>330</v>
+      <c r="C206" t="s">
+        <v>319</v>
+      </c>
+      <c r="J206" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
+      <c r="B207" s="57" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A208" s="13" t="s">
+      <c r="A208" s="13"/>
+      <c r="B208" s="57" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="13"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="13" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A209" s="13" t="s">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C211" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="13"/>
-      <c r="B210" s="58" t="s">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="13"/>
+      <c r="B212" s="57" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A211" s="13"/>
-      <c r="B211" s="58" t="s">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="13"/>
+      <c r="B213" s="57" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="32" t="s">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="B214" s="22"/>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A215" s="32" t="s">
+      <c r="B216" s="21"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="B215" s="22"/>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
+      <c r="B217" s="21"/>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" s="22" t="s">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="21" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" s="22" t="s">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="21" t="s">
         <v>312</v>
       </c>
-      <c r="B219" s="19"/>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A220" s="22" t="s">
+      <c r="B221" s="19"/>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="21" t="s">
         <v>130</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="21"/>
+    </row>
+    <row r="224" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B226" s="58" t="s">
+        <v>346</v>
+      </c>
+      <c r="C226" s="59" t="s">
+        <v>350</v>
+      </c>
+      <c r="D226" s="58" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B228" s="58" t="s">
+        <v>348</v>
+      </c>
+      <c r="C228" s="59" t="s">
+        <v>350</v>
+      </c>
+      <c r="D228" s="58" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B231" s="58" t="s">
+        <v>355</v>
+      </c>
+      <c r="C231" s="59" t="s">
+        <v>350</v>
+      </c>
+      <c r="D231" s="58" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B233" s="58" t="s">
+        <v>348</v>
+      </c>
+      <c r="C233" s="59" t="s">
+        <v>350</v>
+      </c>
+      <c r="D233" s="58" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B236" s="58" t="s">
+        <v>357</v>
+      </c>
+      <c r="C236" s="59" t="s">
+        <v>350</v>
+      </c>
+      <c r="D236" s="58" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="C239" s="59" t="s">
+        <v>350</v>
+      </c>
+      <c r="D239" s="58" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C242" s="59" t="s">
+        <v>350</v>
+      </c>
+      <c r="D242" s="58" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3628,7 +3848,7 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3647,474 +3867,474 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="35" customWidth="1"/>
-    <col min="2" max="2" width="16.375" style="35" customWidth="1"/>
-    <col min="3" max="3" width="59.375" style="35" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="35"/>
+    <col min="1" max="1" width="18.5" style="34" customWidth="1"/>
+    <col min="2" max="2" width="16.375" style="34" customWidth="1"/>
+    <col min="3" max="3" width="59.375" style="34" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>236</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="36"/>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="38" t="s">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="37" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="38" t="s">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="37" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="38" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="37" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="38" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="38" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="B9" s="39"/>
+      <c r="B9" s="38"/>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>245</v>
       </c>
-      <c r="B10" s="40"/>
+      <c r="B10" s="39"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="35" t="s">
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="34" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40" t="s">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40" t="s">
+      <c r="A13" s="39"/>
+      <c r="B13" s="39" t="s">
         <v>230</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="39" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40" t="s">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39" t="s">
         <v>246</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="41" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
     </row>
     <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="37" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="35" t="s">
+      <c r="B21" s="38"/>
+      <c r="C21" s="34" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="38" t="s">
+      <c r="B22" s="38"/>
+      <c r="C22" s="37" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="35" t="s">
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="34" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="38" t="s">
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="37" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="B28" s="37"/>
+      <c r="B28" s="36"/>
     </row>
     <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="37" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="40" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="40" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="40" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="36" t="s">
         <v>238</v>
       </c>
-      <c r="B35" s="37"/>
+      <c r="B35" s="36"/>
     </row>
     <row r="36" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="37" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="47" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="48" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="34" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="34" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="34" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="42" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="48" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+      <c r="A44" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="C44" s="43" t="s">
+      <c r="C44" s="42" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C45" s="43"/>
+      <c r="C45" s="42"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="C46" s="54" t="s">
+      <c r="C46" s="53" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="C47" s="38" t="s">
+      <c r="C47" s="37" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="36" t="s">
         <v>239</v>
       </c>
-      <c r="B49" s="37"/>
+      <c r="B49" s="36"/>
     </row>
     <row r="50" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C50" s="38" t="s">
+      <c r="C50" s="37" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="C52" s="38" t="s">
+      <c r="C52" s="37" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="34" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="37" t="s">
+      <c r="A57" s="36" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="47" t="s">
+      <c r="A58" s="46" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="44" t="s">
+      <c r="A59" s="43" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="47" t="s">
+      <c r="A60" s="46" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="44" t="s">
+      <c r="A61" s="43" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="47" t="s">
+      <c r="A62" s="46" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="44" t="s">
+      <c r="A63" s="43" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="44" t="s">
+      <c r="A64" s="43" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="44" t="s">
+      <c r="A65" s="43" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="45" t="s">
+      <c r="A66" s="44" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="46" t="s">
+      <c r="A67" s="45" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="43" t="s">
+      <c r="B69" s="42" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="43" t="s">
+      <c r="B70" s="42" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="35" t="s">
+      <c r="B71" s="34" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="35" t="s">
+      <c r="B73" s="34" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="35" t="s">
+      <c r="B75" s="34" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="35" t="s">
+      <c r="B76" s="34" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="35" t="s">
+      <c r="B77" s="34" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="53" t="s">
+    <row r="79" spans="1:2" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="52" t="s">
         <v>283</v>
       </c>
-      <c r="B79" s="53" t="s">
+      <c r="B79" s="52" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="81" spans="1:3" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="50" t="s">
+    <row r="81" spans="1:3" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="B81" s="50" t="s">
+      <c r="B81" s="49" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="82" spans="1:3" s="52" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="C82" s="52" t="s">
+    <row r="82" spans="1:3" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="C82" s="51" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="83" spans="1:3" s="52" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="C83" s="52" t="s">
+    <row r="83" spans="1:3" s="51" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="C83" s="51" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="84" spans="1:3" s="52" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="C84" s="52" t="s">
+    <row r="84" spans="1:3" s="51" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="C84" s="51" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="85" spans="1:3" s="52" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="C85" s="52" t="s">
+    <row r="85" spans="1:3" s="51" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="C85" s="51" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="86" spans="1:3" s="50" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="51" t="s">
+    <row r="86" spans="1:3" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="1:3" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="50" t="s">
         <v>286</v>
       </c>
-      <c r="B87" s="51" t="s">
+      <c r="B87" s="50" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="88" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="51" t="s">
+    <row r="88" spans="1:3" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="50" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="35" t="s">
+      <c r="A90" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="B90" s="35" t="s">
+      <c r="B90" s="34" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="35" t="s">
+      <c r="A91" s="34" t="s">
         <v>285</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Collect all call target and call sites parameters at the code element level
</commit_message>
<xml_diff>
--- a/TypeCobol/Documentation/Studies/SymbolInformationsAndStorageAreas.xlsx
+++ b/TypeCobol/Documentation/Studies/SymbolInformationsAndStorageAreas.xlsx
@@ -2528,8 +2528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J242"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="A210" sqref="A210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>